<commit_message>
se limpian datos de plantilla para cargue de productos
</commit_message>
<xml_diff>
--- a/sbx/archivos/Importar/ProductoStock.xlsx
+++ b/sbx/archivos/Importar/ProductoStock.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\Documents\PROYECTOS\SBX\APLICACION ESCRITORIO\Local\archivos\Cargue masivo\Productos con exitencias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\Documents\PROYECTOS\SBX\APLICACION ESCRITORIO\Local\sbx\archivos\Importar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sku</t>
   </si>
@@ -45,21 +45,6 @@
   </si>
   <si>
     <t>Stock *</t>
-  </si>
-  <si>
-    <t>teclado</t>
-  </si>
-  <si>
-    <t>mause</t>
-  </si>
-  <si>
-    <t>puerta</t>
-  </si>
-  <si>
-    <t>hp</t>
-  </si>
-  <si>
-    <t>logict</t>
   </si>
 </sst>
 </file>
@@ -462,7 +447,7 @@
   <dimension ref="A1:G2875"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -498,52 +483,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>42500</v>
-      </c>
-      <c r="G2" s="14">
-        <v>5</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="14">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="14">
-        <v>20000</v>
-      </c>
-      <c r="G3" s="14">
-        <v>10</v>
-      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="14">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14">
-        <v>150000</v>
-      </c>
-      <c r="G4" s="14">
-        <v>4</v>
-      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>

</xml_diff>